<commit_message>
UpdatedDB plus UML added
</commit_message>
<xml_diff>
--- a/Documentation/Project/Database.xlsx
+++ b/Documentation/Project/Database.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tafewa-my.sharepoint.com/personal/j162548_tafe_wa_edu_au/Documents/NFS/Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\William  Te\Desktop\NavyFood\NavyFoodSecurity\Documentation\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="82" documentId="13_ncr:1_{DE18F2E7-05B7-457F-874A-3150C5D7AA22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EF14D82D-A276-4B73-B8EA-78F25576312C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75793D7C-8913-4EC7-B81C-087681D68CCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12780" yWindow="997" windowWidth="15390" windowHeight="9533" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5130" yWindow="997" windowWidth="15390" windowHeight="9533" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="92">
   <si>
     <t>Database</t>
   </si>
@@ -307,6 +307,9 @@
   </si>
   <si>
     <t>locationID</t>
+  </si>
+  <si>
+    <t>DriverId</t>
   </si>
 </sst>
 </file>
@@ -694,7 +697,7 @@
   <dimension ref="A1:M47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G3" workbookViewId="0">
-      <selection activeCell="H29" activeCellId="1" sqref="I19 H29"/>
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -989,6 +992,9 @@
       <c r="G19" s="6" t="s">
         <v>8</v>
       </c>
+      <c r="I19" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="K19" s="1" t="s">
         <v>88</v>
       </c>

</xml_diff>